<commit_message>
Update Touchstone User Flows.xlsx
Flow 12 -16 deleted
</commit_message>
<xml_diff>
--- a/doc/message/common/Touchstone User Flows.xlsx
+++ b/doc/message/common/Touchstone User Flows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ire/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\dk-medcom\dk-medcom\doc\message\common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A55A4F5-9024-3146-8132-0A8D528B310E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5720DFEA-D365-47DC-8E7A-F271A2EB58D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13480" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{C44E6051-BBCE-EE47-A48B-C4FC575873B7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{C44E6051-BBCE-EE47-A48B-C4FC575873B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Send HospitalNotification" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="175">
   <si>
     <t>User Flow:  HospitalNotification - sending messages</t>
   </si>
@@ -84,9 +84,6 @@
     <t>S1 + S3</t>
   </si>
   <si>
-    <t>S1: Provenance.activity.coding.code =  admit-inpatient &amp; Encounter.class.code = IMP &amp; Encounter.status = in-progress  S3: Provenance.activity.coding.code =  discharge-inpatient-home &amp; Encounter.class.code = IMP &amp; Encounter.status = finished || S1 and S3: Encounter.identifier.value equal || S1 and S3: S3.Provenance[2].entity.what.reference refference S1.Bundle.entry[0].fullUrl || S1 and S3 same episodeOfCare.identifier</t>
-  </si>
-  <si>
     <t>https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUS_H_V_1-xml</t>
   </si>
   <si>
@@ -126,18 +123,12 @@
     <t>UF_H_V_8</t>
   </si>
   <si>
-    <t>Error: Patient is admitted at hospital and by mistake a dismiss notitication is sent</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
     <t>UF_H_V_9</t>
   </si>
   <si>
-    <t xml:space="preserve">Correction: The patient is admitted and dismissed, the dismis notification is corrected </t>
-  </si>
-  <si>
     <t>UF_H_V_10</t>
   </si>
   <si>
@@ -162,45 +153,24 @@
     <t>Patient is admitted at hospital, transferred to another department, and finally discharged to home</t>
   </si>
   <si>
-    <t>S1 + S6.1 + S6.2 + S3</t>
-  </si>
-  <si>
     <t>UF_H_V_13</t>
   </si>
   <si>
     <t>Patient is admitted at hospital, transferred to another hospital (same region), and finally discharged to home</t>
   </si>
   <si>
-    <t>S1 + S7.1a (initial hospital) + S7.2 (receiving hospital - corresponds to S1) + S3</t>
-  </si>
-  <si>
     <t>UF_H_V_14</t>
   </si>
   <si>
-    <t>Patient is admitted at hospital, transfers himself to another hospital (same region), and is finally dicharged to home</t>
-  </si>
-  <si>
-    <t>S1 + S7.1b (initial hospital - corresponds to S3) + S7.2 (receiving hospital - corresponds to S1) + S3</t>
-  </si>
-  <si>
     <t>UF_H_V_15</t>
   </si>
   <si>
     <t>Patient is admitted at hospital, transferred to another hospital (another region), and finally discharged to home</t>
   </si>
   <si>
-    <t>S1 + S8.1a (initial hospital) + S8.2 (receiving hospital - corresponds to S1) + S3</t>
-  </si>
-  <si>
     <t>UF_H_V_16</t>
   </si>
   <si>
-    <t>Patient is admitted at hospital, transfers himself to another hospital (another region), and is finally discharged to home</t>
-  </si>
-  <si>
-    <t>S1 + S8.1b (initial hospital - corresponds to S3) + S7.2 (receiving hospital - corresponds to S1) + S3</t>
-  </si>
-  <si>
     <t>UF_H_V_17</t>
   </si>
   <si>
@@ -255,9 +225,6 @@
     <t>K2 + K3</t>
   </si>
   <si>
-    <t>K1 and K3: no validation only receiving of the instances</t>
-  </si>
-  <si>
     <t>K1 + K4 + K5 + K3</t>
   </si>
   <si>
@@ -516,42 +483,9 @@
     <t>/FHIRSandbox/MedCom/401-Hospitalnotification/send/Userstory/UF_H_V_11-xml</t>
   </si>
   <si>
-    <t>S5 er ikke en del af TS testen?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S6.1 der er ingen teknisk action. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient is admitted at hospital, goes on leave from hospital but never returns after leave </t>
-  </si>
-  <si>
-    <t>/FHIRSandbox/MedCom/401-Hospitalnotification/send/Userstory/UF_H_V_12-xml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S7.1a der er ingen teknisk action. </t>
-  </si>
-  <si>
-    <t>/FHIRSandbox/MedCom/401-Hospitalnotification/send/Userstory/UF_H_V_13-xml</t>
-  </si>
-  <si>
-    <t>/FHIRSandbox/MedCom/401-Hospitalnotification/send/Userstory/UF_H_V_14-xml</t>
-  </si>
-  <si>
-    <t>Flow: STIN-NOAction-STIN-SLHJ</t>
-  </si>
-  <si>
-    <t>/FHIRSandbox/MedCom/401-Hospitalnotification/send/Userstory/UF_H_V_15-xml</t>
-  </si>
-  <si>
-    <t>Flow: STIN-SLHJ-STIN-SLHJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">date format as expected </t>
   </si>
   <si>
-    <t>/FHIRSandbox/MedCom/401-Hospitalnotification/send/Userstory/UF_H_V_16-xml-json</t>
-  </si>
-  <si>
     <t>Flow: STAA-STIN</t>
   </si>
   <si>
@@ -571,13 +505,91 @@
   </si>
   <si>
     <t>Flow: STIN-STOR-SLOR-MORS</t>
+  </si>
+  <si>
+    <t>STIN+SLHJ</t>
+  </si>
+  <si>
+    <t>RE_STIN</t>
+  </si>
+  <si>
+    <t>AN_STIN</t>
+  </si>
+  <si>
+    <t>STAA+SLHJ</t>
+  </si>
+  <si>
+    <t>STIN+STOR+SLOR+SLHJ</t>
+  </si>
+  <si>
+    <t>STIN+STOR+SLHJ</t>
+  </si>
+  <si>
+    <t>STIN+STIN+SLHJ</t>
+  </si>
+  <si>
+    <t>STIN+SLHJ+STIN</t>
+  </si>
+  <si>
+    <t>STAA+STIN</t>
+  </si>
+  <si>
+    <t>MORS</t>
+  </si>
+  <si>
+    <t>STIN+MORS</t>
+  </si>
+  <si>
+    <t>STIN+STOR+MORS</t>
+  </si>
+  <si>
+    <t>STIN+</t>
+  </si>
+  <si>
+    <t>UF_H_V_2</t>
+  </si>
+  <si>
+    <t>UF_H_V_3</t>
+  </si>
+  <si>
+    <t>UF_H_V_4</t>
+  </si>
+  <si>
+    <t>STIN14 + RE_STIN14</t>
+  </si>
+  <si>
+    <t>STIN12 + AN_STIN12</t>
+  </si>
+  <si>
+    <t>Patient is admitted at hospital, goes on leave from hospital but never returns after leave and is discharged to home</t>
+  </si>
+  <si>
+    <t>Flow: STIN+STIN</t>
+  </si>
+  <si>
+    <t>Flow:STIN+STIN</t>
+  </si>
+  <si>
+    <t>Flow:STAA+SLHJ</t>
+  </si>
+  <si>
+    <t>Flow:STIN+STOR+SLOR+SLHJ</t>
+  </si>
+  <si>
+    <t>Flow: STIN+STOR+SLHJ</t>
+  </si>
+  <si>
+    <t>() = No message is send</t>
+  </si>
+  <si>
+    <t>Flow: STIN+SLHJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -676,7 +688,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -704,6 +716,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,7 +818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -889,7 +907,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -903,6 +920,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1152,8 +1172,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88EC63B5-05E7-AF4F-AE15-17A9F7873F49}" name="Table1" displayName="Table1" ref="B1:F18" totalsRowShown="0">
-  <autoFilter ref="B1:F18" xr:uid="{E071C102-955A-744D-A54B-1F1078368128}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88EC63B5-05E7-AF4F-AE15-17A9F7873F49}" name="Table1" displayName="Table1" ref="B1:F11" totalsRowShown="0">
+  <autoFilter ref="B1:F11" xr:uid="{E071C102-955A-744D-A54B-1F1078368128}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{24747F76-E519-4844-BDC7-094B4AE1EB90}" name="User Flow:  HospitalNotification - sending messages" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{BC78A344-2D5B-354B-AF0B-0FE173A9E19A}" name=" Use Case id reference"/>
@@ -1529,25 +1549,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC787A2-7547-B548-9818-25F247DD3538}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
-    <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="3" max="3" width="78.58203125" customWidth="1"/>
     <col min="4" max="4" width="87.33203125" customWidth="1"/>
-    <col min="5" max="5" width="100.6640625" customWidth="1"/>
+    <col min="5" max="5" width="100.58203125" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21.5" thickBot="1">
       <c r="A1" s="36" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1565,7 +1585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="35" t="s">
         <v>5</v>
       </c>
@@ -1576,305 +1596,196 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="B3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" thickBot="1">
+      <c r="A6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="C7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>28</v>
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>142</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>154</v>
+    <row r="9" spans="1:6">
+      <c r="A9" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
-        <v>32</v>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>35</v>
+    <row r="11" spans="1:6" ht="16" thickBot="1">
+      <c r="A11" s="38" t="s">
+        <v>46</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>161</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>168</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" s="12"/>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{A476ACA5-F5B8-1748-B492-5B95454DD026}"/>
-    <hyperlink ref="E8" r:id="rId2" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_10-xml&amp;version=24&amp;latestVersion=24" xr:uid="{A1AE8183-C381-4F00-9F59-E9F8CF5C7D72}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_10-xml&amp;version=24&amp;latestVersion=24" xr:uid="{A1AE8183-C381-4F00-9F59-E9F8CF5C7D72}"/>
     <hyperlink ref="E3" r:id="rId3" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_6-xml&amp;version=4&amp;latestVersion=4" xr:uid="{64AD4CF7-B983-4383-90EC-1962A5EB12E4}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{13B30E3A-4259-4339-8370-4C1A6CA3E63F}"/>
     <hyperlink ref="E4" r:id="rId5" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_10-xml&amp;version=24&amp;latestVersion=24" xr:uid="{C600D5E8-F4EC-4A61-B3F3-6B0341BD150E}"/>
-    <hyperlink ref="E9" r:id="rId6" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_11-xml&amp;version=3&amp;latestVersion=3" xr:uid="{6D09CC6C-D9D8-4265-B9FC-66EEB99D439F}"/>
-    <hyperlink ref="E10" r:id="rId7" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_12-xml&amp;version=2&amp;latestVersion=2" xr:uid="{440D1055-F66F-4DC0-A83E-0B3E12A969C9}"/>
-    <hyperlink ref="E11" r:id="rId8" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_13-xml&amp;version=1&amp;latestVersion=1" xr:uid="{9B8F5779-6718-4A0D-AF5E-A5E768E5B213}"/>
-    <hyperlink ref="E12" r:id="rId9" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_14-xml&amp;version=5&amp;latestVersion=5" xr:uid="{601EB08C-DA0D-43F6-8EA5-CD21094A49F3}"/>
-    <hyperlink ref="E13" r:id="rId10" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_15-xml&amp;version=4&amp;latestVersion=4" xr:uid="{432036E0-C15E-464B-BCBD-542555DD5ABB}"/>
-    <hyperlink ref="E14" r:id="rId11" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_16-xml-json&amp;version=2&amp;latestVersion=2" xr:uid="{BCD96457-851D-440D-B6E6-CDA8240DF2EE}"/>
-    <hyperlink ref="E15" r:id="rId12" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_17-xml-json&amp;version=1&amp;latestVersion=1" xr:uid="{598ADBB2-E148-47A7-869B-56E6B43B2A5F}"/>
-    <hyperlink ref="E16" r:id="rId13" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_18-xml-json&amp;version=2&amp;latestVersion=2" xr:uid="{4B2143C0-B481-459F-B134-73BAD8CD6917}"/>
-    <hyperlink ref="E17" r:id="rId14" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_19-xml-json&amp;version=2&amp;latestVersion=2" xr:uid="{4435D2AD-13AA-41CD-B4CB-01649FDED6A8}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_11-xml&amp;version=3&amp;latestVersion=3" xr:uid="{6D09CC6C-D9D8-4265-B9FC-66EEB99D439F}"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_17-xml-json&amp;version=1&amp;latestVersion=1" xr:uid="{598ADBB2-E148-47A7-869B-56E6B43B2A5F}"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_18-xml-json&amp;version=2&amp;latestVersion=2" xr:uid="{4B2143C0-B481-459F-B134-73BAD8CD6917}"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://touchstone.aegis.net/touchstone/testscript?name=%2fFHIRSandbox%2fMedCom%2f401-Hospitalnotification%2fsend%2fUserstory%2fUF_H_V_19-xml-json&amp;version=2&amp;latestVersion=2" xr:uid="{4435D2AD-13AA-41CD-B4CB-01649FDED6A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1887,34 +1798,34 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1929,28 +1840,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D3C847-0C53-D143-A3F1-9F26902134B6}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="110.33203125" customWidth="1"/>
-    <col min="3" max="3" width="158.6640625" customWidth="1"/>
-    <col min="4" max="4" width="165.33203125" customWidth="1"/>
+    <col min="3" max="3" width="67.83203125" customWidth="1"/>
+    <col min="4" max="4" width="68.25" customWidth="1"/>
     <col min="5" max="5" width="185.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1962,177 +1873,259 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="45"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="D11" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="44" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="C12" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="45"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="44" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="C13" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D13" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="D14" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="D15" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="D16" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>80</v>
+      <c r="D17" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2148,25 +2141,25 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="64.1640625" customWidth="1"/>
+    <col min="2" max="2" width="64.08203125" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="58.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -2178,368 +2171,368 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="21">
       <c r="A2" s="19"/>
       <c r="B2" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18" customHeight="1">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="31">
       <c r="A6" s="19"/>
       <c r="B6" s="19" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="21"/>
       <c r="B7" s="21" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="31">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="31">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="31">
       <c r="A10" s="22"/>
       <c r="B10" s="22" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31">
       <c r="A11" s="21"/>
       <c r="B11" s="21" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="19"/>
       <c r="B12" s="19" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="31">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31">
       <c r="A14" s="22"/>
       <c r="B14" s="22" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="22"/>
       <c r="B16" s="22" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="31">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="31">
       <c r="A18" s="25"/>
       <c r="B18" s="25" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31">
       <c r="A19" s="23"/>
       <c r="B19" s="23" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="31"/>
       <c r="B20" s="31" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="29"/>
       <c r="B21" s="29" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="19"/>
       <c r="B22" s="19" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="31">
       <c r="A24" s="22"/>
       <c r="B24" s="22" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="31">
       <c r="A25" s="21"/>
       <c r="B25" s="21" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="31">
       <c r="A26" s="22"/>
       <c r="B26" s="22" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="27"/>
       <c r="B27" s="27" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F27" s="6"/>
     </row>
@@ -2559,24 +2552,24 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.08203125" customWidth="1"/>
+    <col min="5" max="5" width="29.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21.5" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
@@ -2588,68 +2581,68 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
+    <row r="2" spans="1:6">
+      <c r="A2" s="40"/>
       <c r="B2" s="14" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
+    <row r="3" spans="1:6">
+      <c r="A3" s="39"/>
       <c r="B3" s="17" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+    <row r="4" spans="1:6">
+      <c r="A4" s="39"/>
       <c r="B4" s="18" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="39"/>
       <c r="B5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="41"/>
+      <c r="B6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>143</v>
-      </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="13"/>
     </row>
@@ -2663,18 +2656,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2857,6 +2850,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBAD5D2F-F402-4F5F-AC8E-165FE0A9ABFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{614B2C52-CAE6-4EEC-AD7A-7A6E583F3B0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2869,14 +2870,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="f96a63b6-96d6-4a7d-9bdb-373dd23aadd0"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBAD5D2F-F402-4F5F-AC8E-165FE0A9ABFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>